<commit_message>
for #DDDX 2012 conf
</commit_message>
<xml_diff>
--- a/App/Demo.Sln/Demo.Dom.CoffeeShop.Fixtures/Fixtures/CoffeeShop.xlsx
+++ b/App/Demo.Sln/Demo.Dom.CoffeeShop.Fixtures/Fixtures/CoffeeShop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="812" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="812" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>type</t>
   </si>
@@ -62,9 +62,6 @@
     <t>SKU~0002</t>
   </si>
   <si>
-    <t>Cappacinno</t>
-  </si>
-  <si>
     <t>SKU~0003</t>
   </si>
   <si>
@@ -83,12 +80,6 @@
     <t>bit</t>
   </si>
   <si>
-    <t>OrderId</t>
-  </si>
-  <si>
-    <t>uniqueidentifier</t>
-  </si>
-  <si>
     <t>ProductSku</t>
   </si>
   <si>
@@ -117,6 +108,21 @@
   </si>
   <si>
     <t>Addition</t>
+  </si>
+  <si>
+    <t>Cappuccino</t>
+  </si>
+  <si>
+    <t>PlacedOn</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>OrderNum</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -484,17 +490,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -563,10 +569,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -592,7 +598,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,10 +624,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -630,7 +636,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -648,25 +654,25 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -674,7 +680,12 @@
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C8" s="1"/>
     </row>
   </sheetData>
@@ -687,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,10 +725,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -726,7 +737,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -762,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +799,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -810,7 +821,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3">
         <v>3.1</v>
@@ -821,10 +832,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="3">
         <v>2.4</v>
@@ -835,10 +846,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3">
         <v>0.5</v>
@@ -849,10 +860,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
         <v>0.4</v>

</xml_diff>